<commit_message>
Add creator and createddate to article table
Signed-off-by: shadberry <shadberry89@gmail.com>
</commit_message>
<xml_diff>
--- a/Blog Table Information.xlsx
+++ b/Blog Table Information.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="66">
   <si>
     <t>逻辑名称</t>
   </si>
@@ -240,15 +240,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>SUMMARY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>摘要</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATEDUSERID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建者</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>MODIFYDATE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SUMMARY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>摘要</t>
+    <t>MODIFYUSERID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改者</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -327,9 +351,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -346,6 +367,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -710,468 +734,500 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="5.25" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.25" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.75" customWidth="1"/>
     <col min="3" max="3" width="22.625" customWidth="1"/>
     <col min="4" max="4" width="18.125" customWidth="1"/>
     <col min="5" max="5" width="24.25" customWidth="1"/>
-    <col min="6" max="6" width="9" style="7"/>
+    <col min="6" max="6" width="9" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="2" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="3"/>
+      <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>1</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>2</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="6"/>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>3</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="6"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>4</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="6"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>5</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>6</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="6"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="2" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F23" s="3"/>
+      <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>1</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>2</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="6"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>3</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="5" t="s">
+      <c r="E27" s="4"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="3">
+        <v>4</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="3">
+        <v>5</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="3">
+        <v>6</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="4">
-        <v>4</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="5" t="s">
+      <c r="D30" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="3">
         <v>7</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="6"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="4">
-        <v>5</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="5" t="s">
+      <c r="B31" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="6"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="4">
-        <v>6</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="3">
+        <v>8</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
1. Configure Log4j for log. 2. Add jquery library. 3. Modify some POJO because the db table has been changed. 4. Add JDom prepare for parsing sql configuration XML. 5. Add an interceptor to manage session commit and rollback.
Signed-off-by: shadberry <shadberry89@gmail.com>
</commit_message>
<xml_diff>
--- a/Blog Table Information.xlsx
+++ b/Blog Table Information.xlsx
@@ -72,10 +72,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DATE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>NAME</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -252,10 +248,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CREATEDUSERID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>创建者</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -264,15 +256,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MODIFYUSERID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>INT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>修改者</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DATETIME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MODIFIERID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATORID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -736,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -756,13 +756,13 @@
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2"/>
     </row>
@@ -774,7 +774,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -794,7 +794,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
@@ -811,13 +811,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="5"/>
@@ -827,13 +827,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="5"/>
@@ -843,13 +843,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="5"/>
@@ -859,13 +859,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="5"/>
@@ -875,13 +875,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="5"/>
@@ -891,16 +891,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="5"/>
     </row>
@@ -909,13 +909,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="5"/>
@@ -926,13 +926,13 @@
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -964,7 +964,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>11</v>
@@ -981,16 +981,16 @@
         <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F16" s="5"/>
     </row>
@@ -999,13 +999,13 @@
         <v>3</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="5"/>
@@ -1015,13 +1015,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="5"/>
@@ -1031,10 +1031,10 @@
         <v>5</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>8</v>
@@ -1047,13 +1047,13 @@
         <v>6</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="5"/>
@@ -1064,13 +1064,13 @@
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F23" s="2"/>
     </row>
@@ -1102,7 +1102,7 @@
         <v>11</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>11</v>
@@ -1119,13 +1119,13 @@
         <v>2</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="5"/>
@@ -1135,13 +1135,13 @@
         <v>3</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="5"/>
@@ -1151,13 +1151,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="5"/>
@@ -1167,13 +1167,13 @@
         <v>5</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="5"/>
@@ -1183,13 +1183,13 @@
         <v>6</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="5"/>
@@ -1199,13 +1199,13 @@
         <v>7</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="5"/>
@@ -1215,13 +1215,13 @@
         <v>8</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="5"/>

</xml_diff>

<commit_message>
1. Add a comment table to db, generate the O/R mapping file and corresponding DAO, POJO java file. 2. Change the hibernate default dialect class to my custom one to fix the blob problem when query by sql. 3. Add a permisson define xml for the auth verify later. 4. Change list all article function to using sql that configure in XML rather than Hibernate HQL.
Signed-off-by: shadberry <shadberry89@gmail.com>
</commit_message>
<xml_diff>
--- a/Blog Table Information.xlsx
+++ b/Blog Table Information.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
   <si>
     <t>逻辑名称</t>
   </si>
@@ -273,6 +273,34 @@
   </si>
   <si>
     <t>CREATORID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T_COMMENT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>评论表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ARTICLEID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>评论的文档ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以是USER/VISITOR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR2（1000）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -347,7 +375,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -367,6 +395,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -734,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -751,10 +782,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="8"/>
       <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
@@ -921,10 +952,10 @@
       <c r="F10" s="5"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="7"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1059,10 +1090,10 @@
       <c r="F20" s="5"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="7"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="1" t="s">
         <v>48</v>
       </c>
@@ -1226,14 +1257,153 @@
       <c r="E32" s="4"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:6">
       <c r="A33"/>
     </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="3">
+        <v>1</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="3">
+        <v>2</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="3">
+        <v>3</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="3">
+        <v>4</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="3">
+        <v>5</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="3">
+        <v>6</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F42" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A35:B35"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1. Add an article key word db table and it's hibernate files... 2. Add a page which is used for write new article with ckeditor. 3. Finish post new article function.
Signed-off-by: shadberry <shadberry89@gmail.com>
</commit_message>
<xml_diff>
--- a/Blog Table Information.xlsx
+++ b/Blog Table Information.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="79">
   <si>
     <t>逻辑名称</t>
   </si>
@@ -301,6 +301,30 @@
   </si>
   <si>
     <t>VARCHAR2（1000）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T_KEYWORD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关键字表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ARTICLEID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文档ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KEYWORD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关键字</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -375,7 +399,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -395,6 +419,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -765,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47:D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -782,10 +809,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="9"/>
       <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
@@ -952,10 +979,10 @@
       <c r="F10" s="5"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1090,10 +1117,10 @@
       <c r="F20" s="5"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="8"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="1" t="s">
         <v>48</v>
       </c>
@@ -1261,10 +1288,10 @@
       <c r="A33"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="8"/>
+      <c r="B35" s="9"/>
       <c r="C35" s="1" t="s">
         <v>66</v>
       </c>
@@ -1398,12 +1425,103 @@
       </c>
       <c r="F42" s="5"/>
     </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="9"/>
+      <c r="C45" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="3">
+        <v>1</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="3">
+        <v>2</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="3">
+        <v>3</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E49" s="4"/>
+      <c r="F49" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A45:B45"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add a column about read times in article table.
Signed-off-by: shadberry <shadberry89@gmail.com>
</commit_message>
<xml_diff>
--- a/Blog Table Information.xlsx
+++ b/Blog Table Information.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="81">
   <si>
     <t>逻辑名称</t>
   </si>
@@ -325,6 +325,14 @@
   </si>
   <si>
     <t>关键字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>READCOUNT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>读取次数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -792,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47:D49"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1285,243 +1293,259 @@
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="9" t="s">
+      <c r="A33" s="3">
         <v>9</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="1" t="s">
+      <c r="B33" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="9"/>
+      <c r="C36" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="7" t="s">
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F37" s="7" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="3">
-        <v>1</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>72</v>
+        <v>6</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="3">
+        <v>5</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="3">
         <v>6</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B43" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E43" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F42" s="5"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="9" t="s">
+      <c r="F43" s="5"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="1" t="s">
+      <c r="B46" s="9"/>
+      <c r="C46" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F45" s="8"/>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="8" t="s">
+      <c r="F46" s="8"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="8" t="s">
+      <c r="F47" s="8" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="3">
-        <v>1</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>76</v>
+        <v>11</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F48" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="3">
+        <v>2</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="3">
         <v>3</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C50" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D50" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E49" s="4"/>
-      <c r="F49" s="5"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A46:B46"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>